<commit_message>
Second count sample added Signed-off-by: gerrymulvenna <git@movingwifi.com>
</commit_message>
<xml_diff>
--- a/2012/SCO/city-of-edinburgh/S13002924/results.xlsx
+++ b/2012/SCO/city-of-edinburgh/S13002924/results.xlsx
@@ -444,7 +444,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E9" sqref="E9:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,14 +696,22 @@
         <f>"{""Candidate_First_Pref_Votes"":"""&amp;D1&amp;""",""Status"":"""",""Occurred_On_Count"":"""",""Surname"":"""&amp;$B1&amp;""",""Firstname"":"""&amp;$A1&amp;""",""Constituency_Number"":""2"",""Party_Name"":"""&amp;$C1&amp;""",""Candidate_Id"":"""&amp;ROW()&amp;""",""Count_Number"":""1"",""Transfers"":""0.00"",""id"":"&amp;ROW()-9&amp;",""Total_Votes"":"""&amp;D1&amp;"""},"</f>
         <v>{"Candidate_First_Pref_Votes":"2050","Status":"","Occurred_On_Count":"","Surname":"BALFOUR","Firstname":"Jeremy Ross","Constituency_Number":"2","Party_Name":"Scottish Conservative and Unionist","Candidate_Id":"9","Count_Number":"1","Transfers":"0.00","id":0,"Total_Votes":"2050"},</v>
       </c>
+      <c r="E9" t="str">
+        <f>"{""Candidate_First_Pref_Votes"":"""&amp;$D1&amp;""",""Status"":"""",""Occurred_On_Count"":"""",""Surname"":"""&amp;$B1&amp;""",""Firstname"":"""&amp;$A1&amp;""",""Constituency_Number"":""2"",""Party_Name"":"""&amp;$C1&amp;""",""Candidate_Id"":"""&amp;ROW()&amp;""",""Count_Number"":""2"",""Transfers"":"""&amp;E1&amp;""",""id"":"&amp;ROW()-3&amp;",""Total_Votes"":"""&amp;$D1+E1&amp;"""},"</f>
+        <v>{"Candidate_First_Pref_Votes":"2050","Status":"","Occurred_On_Count":"","Surname":"BALFOUR","Firstname":"Jeremy Ross","Constituency_Number":"2","Party_Name":"Scottish Conservative and Unionist","Candidate_Id":"9","Count_Number":"2","Transfers":"50","id":6,"Total_Votes":"2100"},</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" ref="D10:D15" si="0">"{""Candidate_First_Pref_Votes"":"""&amp;D2&amp;""",""Status"":"""",""Occurred_On_Count"":"""",""Surname"":"""&amp;$B2&amp;""",""Firstname"":"""&amp;$A2&amp;""",""Constituency_Number"":""2"",""Party_Name"":"""&amp;$C2&amp;""",""Candidate_Id"":"""&amp;ROW()&amp;""",""Count_Number"":""1"",""Transfers"":""0.00"",""id"":"&amp;ROW()-9&amp;",""Total_Votes"":"""&amp;D2&amp;"""},"</f>
+        <f t="shared" ref="D10:E14" si="0">"{""Candidate_First_Pref_Votes"":"""&amp;D2&amp;""",""Status"":"""",""Occurred_On_Count"":"""",""Surname"":"""&amp;$B2&amp;""",""Firstname"":"""&amp;$A2&amp;""",""Constituency_Number"":""2"",""Party_Name"":"""&amp;$C2&amp;""",""Candidate_Id"":"""&amp;ROW()&amp;""",""Count_Number"":""1"",""Transfers"":""0.00"",""id"":"&amp;ROW()-9&amp;",""Total_Votes"":"""&amp;D2&amp;"""},"</f>
         <v>{"Candidate_First_Pref_Votes":"1788","Status":"","Occurred_On_Count":"","Surname":"EDIE","Firstname":"Paul","Constituency_Number":"2","Party_Name":"Scottish Liberal Democrats","Candidate_Id":"10","Count_Number":"1","Transfers":"0.00","id":1,"Total_Votes":"1788"},</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" ref="E10:E14" si="1">"{""Candidate_First_Pref_Votes"":"""&amp;$D2&amp;""",""Status"":"""",""Occurred_On_Count"":"""",""Surname"":"""&amp;$B2&amp;""",""Firstname"":"""&amp;$A2&amp;""",""Constituency_Number"":""2"",""Party_Name"":"""&amp;$C2&amp;""",""Candidate_Id"":"""&amp;ROW()&amp;""",""Count_Number"":""2"",""Transfers"":"""&amp;E2&amp;""",""id"":"&amp;ROW()-3&amp;",""Total_Votes"":"""&amp;$D2+E2&amp;"""},"</f>
+        <v>{"Candidate_First_Pref_Votes":"1788","Status":"","Occurred_On_Count":"","Surname":"EDIE","Firstname":"Paul","Constituency_Number":"2","Party_Name":"Scottish Liberal Democrats","Candidate_Id":"10","Count_Number":"2","Transfers":"10","id":7,"Total_Votes":"1798"},</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -714,6 +722,10 @@
         <f t="shared" si="0"/>
         <v>{"Candidate_First_Pref_Votes":"502","Status":"","Occurred_On_Count":"","Surname":"HINDE","Firstname":"Dominic","Constituency_Number":"2","Party_Name":"Scottish Green Party","Candidate_Id":"11","Count_Number":"1","Transfers":"0.00","id":2,"Total_Votes":"502"},</v>
       </c>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>{"Candidate_First_Pref_Votes":"502","Status":"","Occurred_On_Count":"","Surname":"HINDE","Firstname":"Dominic","Constituency_Number":"2","Party_Name":"Scottish Green Party","Candidate_Id":"11","Count_Number":"2","Transfers":"24","id":8,"Total_Votes":"526"},</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -723,6 +735,10 @@
         <f t="shared" si="0"/>
         <v>{"Candidate_First_Pref_Votes":"1679","Status":"","Occurred_On_Count":"","Surname":"MCINALLY","Firstname":"Tom","Constituency_Number":"2","Party_Name":"Scottish Labour Party","Candidate_Id":"12","Count_Number":"1","Transfers":"0.00","id":3,"Total_Votes":"1679"},</v>
       </c>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>{"Candidate_First_Pref_Votes":"1679","Status":"","Occurred_On_Count":"","Surname":"MCINALLY","Firstname":"Tom","Constituency_Number":"2","Party_Name":"Scottish Labour Party","Candidate_Id":"12","Count_Number":"2","Transfers":"19","id":9,"Total_Votes":"1698"},</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -732,6 +748,10 @@
         <f t="shared" si="0"/>
         <v>{"Candidate_First_Pref_Votes":"161","Status":"","Occurred_On_Count":"","Surname":"NISBET","Firstname":"James","Constituency_Number":"2","Party_Name":"UK Independence Party (UKIP)","Candidate_Id":"13","Count_Number":"1","Transfers":"0.00","id":4,"Total_Votes":"161"},</v>
       </c>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>{"Candidate_First_Pref_Votes":"161","Status":"","Occurred_On_Count":"","Surname":"NISBET","Firstname":"James","Constituency_Number":"2","Party_Name":"UK Independence Party (UKIP)","Candidate_Id":"13","Count_Number":"2","Transfers":"-161","id":10,"Total_Votes":"0"},</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -740,6 +760,10 @@
       <c r="D14" t="str">
         <f t="shared" si="0"/>
         <v>{"Candidate_First_Pref_Votes":"2032","Status":"","Occurred_On_Count":"","Surname":"ROSS","Firstname":"Frank","Constituency_Number":"2","Party_Name":"Scottish National Party (SNP)","Candidate_Id":"14","Count_Number":"1","Transfers":"0.00","id":5,"Total_Votes":"2032"},</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>{"Candidate_First_Pref_Votes":"2032","Status":"","Occurred_On_Count":"","Surname":"ROSS","Firstname":"Frank","Constituency_Number":"2","Party_Name":"Scottish National Party (SNP)","Candidate_Id":"14","Count_Number":"2","Transfers":"21","id":11,"Total_Votes":"2053"},</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
counts 3 and 4 added Signed-off-by: gerrymulvenna <git@movingwifi.com>
</commit_message>
<xml_diff>
--- a/2012/SCO/city-of-edinburgh/S13002924/results.xlsx
+++ b/2012/SCO/city-of-edinburgh/S13002924/results.xlsx
@@ -24,18 +24,12 @@
     <t>BALFOUR</t>
   </si>
   <si>
-    <t>Scottish Conservative and Unionist</t>
-  </si>
-  <si>
     <t>Paul</t>
   </si>
   <si>
     <t>EDIE</t>
   </si>
   <si>
-    <t>Scottish Liberal Democrats</t>
-  </si>
-  <si>
     <t>Dominic</t>
   </si>
   <si>
@@ -51,9 +45,6 @@
     <t>MCINALLY</t>
   </si>
   <si>
-    <t>Scottish Labour Party</t>
-  </si>
-  <si>
     <t>James</t>
   </si>
   <si>
@@ -103,6 +94,15 @@
   </si>
   <si>
     <t xml:space="preserve">    "id": 0, </t>
+  </si>
+  <si>
+    <t>Conservative and Unionist Party</t>
+  </si>
+  <si>
+    <t>Liberal Democrats</t>
+  </si>
+  <si>
+    <t>Labour Party</t>
   </si>
 </sst>
 </file>
@@ -444,7 +444,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:E14"/>
+      <selection activeCell="K9" sqref="K9:K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,7 +462,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D1">
         <v>2050</v>
@@ -500,13 +500,13 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="D2">
         <v>1788</v>
@@ -544,13 +544,13 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
       <c r="D3">
         <v>502</v>
@@ -582,13 +582,13 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D4">
         <v>1679</v>
@@ -626,13 +626,13 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D5">
         <v>161</v>
@@ -646,13 +646,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D6">
         <v>2032</v>
@@ -690,33 +690,49 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D9" t="str">
         <f>"{""Candidate_First_Pref_Votes"":"""&amp;D1&amp;""",""Status"":"""",""Occurred_On_Count"":"""",""Surname"":"""&amp;$B1&amp;""",""Firstname"":"""&amp;$A1&amp;""",""Constituency_Number"":""2"",""Party_Name"":"""&amp;$C1&amp;""",""Candidate_Id"":"""&amp;ROW()&amp;""",""Count_Number"":""1"",""Transfers"":""0.00"",""id"":"&amp;ROW()-9&amp;",""Total_Votes"":"""&amp;D1&amp;"""},"</f>
-        <v>{"Candidate_First_Pref_Votes":"2050","Status":"","Occurred_On_Count":"","Surname":"BALFOUR","Firstname":"Jeremy Ross","Constituency_Number":"2","Party_Name":"Scottish Conservative and Unionist","Candidate_Id":"9","Count_Number":"1","Transfers":"0.00","id":0,"Total_Votes":"2050"},</v>
+        <v>{"Candidate_First_Pref_Votes":"2050","Status":"","Occurred_On_Count":"","Surname":"BALFOUR","Firstname":"Jeremy Ross","Constituency_Number":"2","Party_Name":"Conservative and Unionist Party","Candidate_Id":"9","Count_Number":"1","Transfers":"0.00","id":0,"Total_Votes":"2050"},</v>
       </c>
       <c r="E9" t="str">
         <f>"{""Candidate_First_Pref_Votes"":"""&amp;$D1&amp;""",""Status"":"""",""Occurred_On_Count"":"""",""Surname"":"""&amp;$B1&amp;""",""Firstname"":"""&amp;$A1&amp;""",""Constituency_Number"":""2"",""Party_Name"":"""&amp;$C1&amp;""",""Candidate_Id"":"""&amp;ROW()&amp;""",""Count_Number"":""2"",""Transfers"":"""&amp;E1&amp;""",""id"":"&amp;ROW()-3&amp;",""Total_Votes"":"""&amp;$D1+E1&amp;"""},"</f>
-        <v>{"Candidate_First_Pref_Votes":"2050","Status":"","Occurred_On_Count":"","Surname":"BALFOUR","Firstname":"Jeremy Ross","Constituency_Number":"2","Party_Name":"Scottish Conservative and Unionist","Candidate_Id":"9","Count_Number":"2","Transfers":"50","id":6,"Total_Votes":"2100"},</v>
+        <v>{"Candidate_First_Pref_Votes":"2050","Status":"","Occurred_On_Count":"","Surname":"BALFOUR","Firstname":"Jeremy Ross","Constituency_Number":"2","Party_Name":"Conservative and Unionist Party","Candidate_Id":"9","Count_Number":"2","Transfers":"50","id":6,"Total_Votes":"2100"},</v>
+      </c>
+      <c r="G9" t="str">
+        <f>"{""Candidate_First_Pref_Votes"":"""&amp;$D1&amp;""",""Status"":"""",""Occurred_On_Count"":"""",""Surname"":"""&amp;$B1&amp;""",""Firstname"":"""&amp;$A1&amp;""",""Constituency_Number"":""2"",""Party_Name"":"""&amp;$C1&amp;""",""Candidate_Id"":"""&amp;ROW()&amp;""",""Count_Number"":""3"",""Transfers"":"""&amp;G1&amp;""",""id"":"&amp;ROW()+6&amp;",""Total_Votes"":"""&amp;$H1&amp;"""},"</f>
+        <v>{"Candidate_First_Pref_Votes":"2050","Status":"","Occurred_On_Count":"","Surname":"BALFOUR","Firstname":"Jeremy Ross","Constituency_Number":"2","Party_Name":"Conservative and Unionist Party","Candidate_Id":"9","Count_Number":"3","Transfers":"-46","id":15,"Total_Votes":"2054"},</v>
+      </c>
+      <c r="K9" t="str">
+        <f>"{""Candidate_First_Pref_Votes"":"""&amp;$D1&amp;""",""Status"":"""",""Occurred_On_Count"":"""",""Surname"":"""&amp;$B1&amp;""",""Firstname"":"""&amp;$A1&amp;""",""Constituency_Number"":""2"",""Party_Name"":"""&amp;$C1&amp;""",""Candidate_Id"":"""&amp;ROW()&amp;""",""Count_Number"":""5"",""Transfers"":"""&amp;K1&amp;""",""id"":"&amp;ROW()+12&amp;",""Total_Votes"":"""&amp;L1&amp;"""},"</f>
+        <v>{"Candidate_First_Pref_Votes":"2050","Status":"","Occurred_On_Count":"","Surname":"BALFOUR","Firstname":"Jeremy Ross","Constituency_Number":"2","Party_Name":"Conservative and Unionist Party","Candidate_Id":"9","Count_Number":"5","Transfers":"0","id":21,"Total_Votes":"2054"},</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" ref="D10:E14" si="0">"{""Candidate_First_Pref_Votes"":"""&amp;D2&amp;""",""Status"":"""",""Occurred_On_Count"":"""",""Surname"":"""&amp;$B2&amp;""",""Firstname"":"""&amp;$A2&amp;""",""Constituency_Number"":""2"",""Party_Name"":"""&amp;$C2&amp;""",""Candidate_Id"":"""&amp;ROW()&amp;""",""Count_Number"":""1"",""Transfers"":""0.00"",""id"":"&amp;ROW()-9&amp;",""Total_Votes"":"""&amp;D2&amp;"""},"</f>
-        <v>{"Candidate_First_Pref_Votes":"1788","Status":"","Occurred_On_Count":"","Surname":"EDIE","Firstname":"Paul","Constituency_Number":"2","Party_Name":"Scottish Liberal Democrats","Candidate_Id":"10","Count_Number":"1","Transfers":"0.00","id":1,"Total_Votes":"1788"},</v>
+        <f t="shared" ref="D10:D14" si="0">"{""Candidate_First_Pref_Votes"":"""&amp;D2&amp;""",""Status"":"""",""Occurred_On_Count"":"""",""Surname"":"""&amp;$B2&amp;""",""Firstname"":"""&amp;$A2&amp;""",""Constituency_Number"":""2"",""Party_Name"":"""&amp;$C2&amp;""",""Candidate_Id"":"""&amp;ROW()&amp;""",""Count_Number"":""1"",""Transfers"":""0.00"",""id"":"&amp;ROW()-9&amp;",""Total_Votes"":"""&amp;D2&amp;"""},"</f>
+        <v>{"Candidate_First_Pref_Votes":"1788","Status":"","Occurred_On_Count":"","Surname":"EDIE","Firstname":"Paul","Constituency_Number":"2","Party_Name":"Liberal Democrats","Candidate_Id":"10","Count_Number":"1","Transfers":"0.00","id":1,"Total_Votes":"1788"},</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" ref="E10:E14" si="1">"{""Candidate_First_Pref_Votes"":"""&amp;$D2&amp;""",""Status"":"""",""Occurred_On_Count"":"""",""Surname"":"""&amp;$B2&amp;""",""Firstname"":"""&amp;$A2&amp;""",""Constituency_Number"":""2"",""Party_Name"":"""&amp;$C2&amp;""",""Candidate_Id"":"""&amp;ROW()&amp;""",""Count_Number"":""2"",""Transfers"":"""&amp;E2&amp;""",""id"":"&amp;ROW()-3&amp;",""Total_Votes"":"""&amp;$D2+E2&amp;"""},"</f>
-        <v>{"Candidate_First_Pref_Votes":"1788","Status":"","Occurred_On_Count":"","Surname":"EDIE","Firstname":"Paul","Constituency_Number":"2","Party_Name":"Scottish Liberal Democrats","Candidate_Id":"10","Count_Number":"2","Transfers":"10","id":7,"Total_Votes":"1798"},</v>
+        <v>{"Candidate_First_Pref_Votes":"1788","Status":"","Occurred_On_Count":"","Surname":"EDIE","Firstname":"Paul","Constituency_Number":"2","Party_Name":"Liberal Democrats","Candidate_Id":"10","Count_Number":"2","Transfers":"10","id":7,"Total_Votes":"1798"},</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" ref="G10:G14" si="2">"{""Candidate_First_Pref_Votes"":"""&amp;$D2&amp;""",""Status"":"""",""Occurred_On_Count"":"""",""Surname"":"""&amp;$B2&amp;""",""Firstname"":"""&amp;$A2&amp;""",""Constituency_Number"":""2"",""Party_Name"":"""&amp;$C2&amp;""",""Candidate_Id"":"""&amp;ROW()&amp;""",""Count_Number"":""3"",""Transfers"":"""&amp;G2&amp;""",""id"":"&amp;ROW()+6&amp;",""Total_Votes"":"""&amp;$H2&amp;"""},"</f>
+        <v>{"Candidate_First_Pref_Votes":"1788","Status":"","Occurred_On_Count":"","Surname":"EDIE","Firstname":"Paul","Constituency_Number":"2","Party_Name":"Liberal Democrats","Candidate_Id":"10","Count_Number":"3","Transfers":"19.4691","id":16,"Total_Votes":"1817.4691"},</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" ref="K10:K14" si="3">"{""Candidate_First_Pref_Votes"":"""&amp;$D2&amp;""",""Status"":"""",""Occurred_On_Count"":"""",""Surname"":"""&amp;$B2&amp;""",""Firstname"":"""&amp;$A2&amp;""",""Constituency_Number"":""2"",""Party_Name"":"""&amp;$C2&amp;""",""Candidate_Id"":"""&amp;ROW()&amp;""",""Count_Number"":""5"",""Transfers"":"""&amp;K2&amp;""",""id"":"&amp;ROW()+6&amp;",""Total_Votes"":"""&amp;L2&amp;"""},"</f>
+        <v>{"Candidate_First_Pref_Votes":"1788","Status":"","Occurred_On_Count":"","Surname":"EDIE","Firstname":"Paul","Constituency_Number":"2","Party_Name":"Liberal Democrats","Candidate_Id":"10","Count_Number":"5","Transfers":"175.29387","id":16,"Total_Votes":"1993.13855"},</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
@@ -726,23 +742,39 @@
         <f t="shared" si="1"/>
         <v>{"Candidate_First_Pref_Votes":"502","Status":"","Occurred_On_Count":"","Surname":"HINDE","Firstname":"Dominic","Constituency_Number":"2","Party_Name":"Scottish Green Party","Candidate_Id":"11","Count_Number":"2","Transfers":"24","id":8,"Total_Votes":"526"},</v>
       </c>
+      <c r="G11" t="str">
+        <f t="shared" si="2"/>
+        <v>{"Candidate_First_Pref_Votes":"502","Status":"","Occurred_On_Count":"","Surname":"HINDE","Firstname":"Dominic","Constituency_Number":"2","Party_Name":"Scottish Green Party","Candidate_Id":"11","Count_Number":"3","Transfers":"4.0515","id":17,"Total_Votes":"530.0515"},</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="3"/>
+        <v>{"Candidate_First_Pref_Votes":"502","Status":"","Occurred_On_Count":"","Surname":"HINDE","Firstname":"Dominic","Constituency_Number":"2","Party_Name":"Scottish Green Party","Candidate_Id":"11","Count_Number":"5","Transfers":"-530.49988","id":17,"Total_Votes":"0"},</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>{"Candidate_First_Pref_Votes":"1679","Status":"","Occurred_On_Count":"","Surname":"MCINALLY","Firstname":"Tom","Constituency_Number":"2","Party_Name":"Scottish Labour Party","Candidate_Id":"12","Count_Number":"1","Transfers":"0.00","id":3,"Total_Votes":"1679"},</v>
+        <v>{"Candidate_First_Pref_Votes":"1679","Status":"","Occurred_On_Count":"","Surname":"MCINALLY","Firstname":"Tom","Constituency_Number":"2","Party_Name":"Labour Party","Candidate_Id":"12","Count_Number":"1","Transfers":"0.00","id":3,"Total_Votes":"1679"},</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="1"/>
-        <v>{"Candidate_First_Pref_Votes":"1679","Status":"","Occurred_On_Count":"","Surname":"MCINALLY","Firstname":"Tom","Constituency_Number":"2","Party_Name":"Scottish Labour Party","Candidate_Id":"12","Count_Number":"2","Transfers":"19","id":9,"Total_Votes":"1698"},</v>
+        <v>{"Candidate_First_Pref_Votes":"1679","Status":"","Occurred_On_Count":"","Surname":"MCINALLY","Firstname":"Tom","Constituency_Number":"2","Party_Name":"Labour Party","Candidate_Id":"12","Count_Number":"2","Transfers":"19","id":9,"Total_Votes":"1698"},</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="2"/>
+        <v>{"Candidate_First_Pref_Votes":"1679","Status":"","Occurred_On_Count":"","Surname":"MCINALLY","Firstname":"Tom","Constituency_Number":"2","Party_Name":"Labour Party","Candidate_Id":"12","Count_Number":"3","Transfers":"3.942","id":18,"Total_Votes":"1701.942"},</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="3"/>
+        <v>{"Candidate_First_Pref_Votes":"1679","Status":"","Occurred_On_Count":"","Surname":"MCINALLY","Firstname":"Tom","Constituency_Number":"2","Party_Name":"Labour Party","Candidate_Id":"12","Count_Number":"5","Transfers":"181.55373","id":18,"Total_Votes":"1883.86526"},</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
@@ -752,10 +784,18 @@
         <f t="shared" si="1"/>
         <v>{"Candidate_First_Pref_Votes":"161","Status":"","Occurred_On_Count":"","Surname":"NISBET","Firstname":"James","Constituency_Number":"2","Party_Name":"UK Independence Party (UKIP)","Candidate_Id":"13","Count_Number":"2","Transfers":"-161","id":10,"Total_Votes":"0"},</v>
       </c>
+      <c r="G13" t="str">
+        <f t="shared" si="2"/>
+        <v>{"Candidate_First_Pref_Votes":"161","Status":"","Occurred_On_Count":"","Surname":"NISBET","Firstname":"James","Constituency_Number":"2","Party_Name":"UK Independence Party (UKIP)","Candidate_Id":"13","Count_Number":"3","Transfers":"","id":19,"Total_Votes":""},</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="3"/>
+        <v>{"Candidate_First_Pref_Votes":"161","Status":"","Occurred_On_Count":"","Surname":"NISBET","Firstname":"James","Constituency_Number":"2","Party_Name":"UK Independence Party (UKIP)","Candidate_Id":"13","Count_Number":"5","Transfers":"","id":19,"Total_Votes":""},</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
@@ -765,30 +805,38 @@
         <f t="shared" si="1"/>
         <v>{"Candidate_First_Pref_Votes":"2032","Status":"","Occurred_On_Count":"","Surname":"ROSS","Firstname":"Frank","Constituency_Number":"2","Party_Name":"Scottish National Party (SNP)","Candidate_Id":"14","Count_Number":"2","Transfers":"21","id":11,"Total_Votes":"2053"},</v>
       </c>
+      <c r="G14" t="str">
+        <f t="shared" si="2"/>
+        <v>{"Candidate_First_Pref_Votes":"2032","Status":"","Occurred_On_Count":"","Surname":"ROSS","Firstname":"Frank","Constituency_Number":"2","Party_Name":"Scottish National Party (SNP)","Candidate_Id":"14","Count_Number":"3","Transfers":"2.7156","id":20,"Total_Votes":"2055.7156"},</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="3"/>
+        <v>{"Candidate_First_Pref_Votes":"2032","Status":"","Occurred_On_Count":"","Surname":"ROSS","Firstname":"Frank","Constituency_Number":"2","Party_Name":"Scottish National Party (SNP)","Candidate_Id":"14","Count_Number":"5","Transfers":"0","id":20,"Total_Votes":"2054"},</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correction on 3 & 4 stages Signed-off-by: gerrymulvenna <git@movingwifi.com>
</commit_message>
<xml_diff>
--- a/2012/SCO/city-of-edinburgh/S13002924/results.xlsx
+++ b/2012/SCO/city-of-edinburgh/S13002924/results.xlsx
@@ -701,12 +701,12 @@
         <v>{"Candidate_First_Pref_Votes":"2050","Status":"","Occurred_On_Count":"","Surname":"BALFOUR","Firstname":"Jeremy Ross","Constituency_Number":"2","Party_Name":"Conservative and Unionist Party","Candidate_Id":"9","Count_Number":"2","Transfers":"50","id":6,"Total_Votes":"2100"},</v>
       </c>
       <c r="G9" t="str">
-        <f>"{""Candidate_First_Pref_Votes"":"""&amp;$D1&amp;""",""Status"":"""",""Occurred_On_Count"":"""",""Surname"":"""&amp;$B1&amp;""",""Firstname"":"""&amp;$A1&amp;""",""Constituency_Number"":""2"",""Party_Name"":"""&amp;$C1&amp;""",""Candidate_Id"":"""&amp;ROW()&amp;""",""Count_Number"":""3"",""Transfers"":"""&amp;G1&amp;""",""id"":"&amp;ROW()+6&amp;",""Total_Votes"":"""&amp;$H1&amp;"""},"</f>
-        <v>{"Candidate_First_Pref_Votes":"2050","Status":"","Occurred_On_Count":"","Surname":"BALFOUR","Firstname":"Jeremy Ross","Constituency_Number":"2","Party_Name":"Conservative and Unionist Party","Candidate_Id":"9","Count_Number":"3","Transfers":"-46","id":15,"Total_Votes":"2054"},</v>
+        <f>"{""Candidate_First_Pref_Votes"":"""&amp;$D1&amp;""",""Status"":"""",""Occurred_On_Count"":"""",""Surname"":"""&amp;$B1&amp;""",""Firstname"":"""&amp;$A1&amp;""",""Constituency_Number"":""2"",""Party_Name"":"""&amp;$C1&amp;""",""Candidate_Id"":"""&amp;ROW()&amp;""",""Count_Number"":""3"",""Transfers"":"""&amp;G1&amp;""",""id"":"&amp;ROW()+3&amp;",""Total_Votes"":"""&amp;$H1&amp;"""},"</f>
+        <v>{"Candidate_First_Pref_Votes":"2050","Status":"","Occurred_On_Count":"","Surname":"BALFOUR","Firstname":"Jeremy Ross","Constituency_Number":"2","Party_Name":"Conservative and Unionist Party","Candidate_Id":"9","Count_Number":"3","Transfers":"-46","id":12,"Total_Votes":"2054"},</v>
       </c>
       <c r="K9" t="str">
-        <f>"{""Candidate_First_Pref_Votes"":"""&amp;$D1&amp;""",""Status"":"""",""Occurred_On_Count"":"""",""Surname"":"""&amp;$B1&amp;""",""Firstname"":"""&amp;$A1&amp;""",""Constituency_Number"":""2"",""Party_Name"":"""&amp;$C1&amp;""",""Candidate_Id"":"""&amp;ROW()&amp;""",""Count_Number"":""5"",""Transfers"":"""&amp;K1&amp;""",""id"":"&amp;ROW()+12&amp;",""Total_Votes"":"""&amp;L1&amp;"""},"</f>
-        <v>{"Candidate_First_Pref_Votes":"2050","Status":"","Occurred_On_Count":"","Surname":"BALFOUR","Firstname":"Jeremy Ross","Constituency_Number":"2","Party_Name":"Conservative and Unionist Party","Candidate_Id":"9","Count_Number":"5","Transfers":"0","id":21,"Total_Votes":"2054"},</v>
+        <f>"{""Candidate_First_Pref_Votes"":"""&amp;$D1&amp;""",""Status"":"""",""Occurred_On_Count"":"""",""Surname"":"""&amp;$B1&amp;""",""Firstname"":"""&amp;$A1&amp;""",""Constituency_Number"":""2"",""Party_Name"":"""&amp;$C1&amp;""",""Candidate_Id"":"""&amp;ROW()&amp;""",""Count_Number"":""4"",""Transfers"":"""&amp;K1&amp;""",""id"":"&amp;ROW()+9&amp;",""Total_Votes"":"""&amp;L1&amp;"""},"</f>
+        <v>{"Candidate_First_Pref_Votes":"2050","Status":"","Occurred_On_Count":"","Surname":"BALFOUR","Firstname":"Jeremy Ross","Constituency_Number":"2","Party_Name":"Conservative and Unionist Party","Candidate_Id":"9","Count_Number":"4","Transfers":"0","id":18,"Total_Votes":"2054"},</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -722,12 +722,12 @@
         <v>{"Candidate_First_Pref_Votes":"1788","Status":"","Occurred_On_Count":"","Surname":"EDIE","Firstname":"Paul","Constituency_Number":"2","Party_Name":"Liberal Democrats","Candidate_Id":"10","Count_Number":"2","Transfers":"10","id":7,"Total_Votes":"1798"},</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" ref="G10:G14" si="2">"{""Candidate_First_Pref_Votes"":"""&amp;$D2&amp;""",""Status"":"""",""Occurred_On_Count"":"""",""Surname"":"""&amp;$B2&amp;""",""Firstname"":"""&amp;$A2&amp;""",""Constituency_Number"":""2"",""Party_Name"":"""&amp;$C2&amp;""",""Candidate_Id"":"""&amp;ROW()&amp;""",""Count_Number"":""3"",""Transfers"":"""&amp;G2&amp;""",""id"":"&amp;ROW()+6&amp;",""Total_Votes"":"""&amp;$H2&amp;"""},"</f>
-        <v>{"Candidate_First_Pref_Votes":"1788","Status":"","Occurred_On_Count":"","Surname":"EDIE","Firstname":"Paul","Constituency_Number":"2","Party_Name":"Liberal Democrats","Candidate_Id":"10","Count_Number":"3","Transfers":"19.4691","id":16,"Total_Votes":"1817.4691"},</v>
+        <f t="shared" ref="G10:G14" si="2">"{""Candidate_First_Pref_Votes"":"""&amp;$D2&amp;""",""Status"":"""",""Occurred_On_Count"":"""",""Surname"":"""&amp;$B2&amp;""",""Firstname"":"""&amp;$A2&amp;""",""Constituency_Number"":""2"",""Party_Name"":"""&amp;$C2&amp;""",""Candidate_Id"":"""&amp;ROW()&amp;""",""Count_Number"":""3"",""Transfers"":"""&amp;G2&amp;""",""id"":"&amp;ROW()+3&amp;",""Total_Votes"":"""&amp;$H2&amp;"""},"</f>
+        <v>{"Candidate_First_Pref_Votes":"1788","Status":"","Occurred_On_Count":"","Surname":"EDIE","Firstname":"Paul","Constituency_Number":"2","Party_Name":"Liberal Democrats","Candidate_Id":"10","Count_Number":"3","Transfers":"19.4691","id":13,"Total_Votes":"1817.4691"},</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" ref="K10:K14" si="3">"{""Candidate_First_Pref_Votes"":"""&amp;$D2&amp;""",""Status"":"""",""Occurred_On_Count"":"""",""Surname"":"""&amp;$B2&amp;""",""Firstname"":"""&amp;$A2&amp;""",""Constituency_Number"":""2"",""Party_Name"":"""&amp;$C2&amp;""",""Candidate_Id"":"""&amp;ROW()&amp;""",""Count_Number"":""5"",""Transfers"":"""&amp;K2&amp;""",""id"":"&amp;ROW()+6&amp;",""Total_Votes"":"""&amp;L2&amp;"""},"</f>
-        <v>{"Candidate_First_Pref_Votes":"1788","Status":"","Occurred_On_Count":"","Surname":"EDIE","Firstname":"Paul","Constituency_Number":"2","Party_Name":"Liberal Democrats","Candidate_Id":"10","Count_Number":"5","Transfers":"175.29387","id":16,"Total_Votes":"1993.13855"},</v>
+        <f t="shared" ref="K10:K14" si="3">"{""Candidate_First_Pref_Votes"":"""&amp;$D2&amp;""",""Status"":"""",""Occurred_On_Count"":"""",""Surname"":"""&amp;$B2&amp;""",""Firstname"":"""&amp;$A2&amp;""",""Constituency_Number"":""2"",""Party_Name"":"""&amp;$C2&amp;""",""Candidate_Id"":"""&amp;ROW()&amp;""",""Count_Number"":""4"",""Transfers"":"""&amp;K2&amp;""",""id"":"&amp;ROW()+9&amp;",""Total_Votes"":"""&amp;L2&amp;"""},"</f>
+        <v>{"Candidate_First_Pref_Votes":"1788","Status":"","Occurred_On_Count":"","Surname":"EDIE","Firstname":"Paul","Constituency_Number":"2","Party_Name":"Liberal Democrats","Candidate_Id":"10","Count_Number":"4","Transfers":"175.29387","id":19,"Total_Votes":"1993.13855"},</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -744,11 +744,11 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="2"/>
-        <v>{"Candidate_First_Pref_Votes":"502","Status":"","Occurred_On_Count":"","Surname":"HINDE","Firstname":"Dominic","Constituency_Number":"2","Party_Name":"Scottish Green Party","Candidate_Id":"11","Count_Number":"3","Transfers":"4.0515","id":17,"Total_Votes":"530.0515"},</v>
+        <v>{"Candidate_First_Pref_Votes":"502","Status":"","Occurred_On_Count":"","Surname":"HINDE","Firstname":"Dominic","Constituency_Number":"2","Party_Name":"Scottish Green Party","Candidate_Id":"11","Count_Number":"3","Transfers":"4.0515","id":14,"Total_Votes":"530.0515"},</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="3"/>
-        <v>{"Candidate_First_Pref_Votes":"502","Status":"","Occurred_On_Count":"","Surname":"HINDE","Firstname":"Dominic","Constituency_Number":"2","Party_Name":"Scottish Green Party","Candidate_Id":"11","Count_Number":"5","Transfers":"-530.49988","id":17,"Total_Votes":"0"},</v>
+        <v>{"Candidate_First_Pref_Votes":"502","Status":"","Occurred_On_Count":"","Surname":"HINDE","Firstname":"Dominic","Constituency_Number":"2","Party_Name":"Scottish Green Party","Candidate_Id":"11","Count_Number":"4","Transfers":"-530.49988","id":20,"Total_Votes":"0"},</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -765,11 +765,11 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" si="2"/>
-        <v>{"Candidate_First_Pref_Votes":"1679","Status":"","Occurred_On_Count":"","Surname":"MCINALLY","Firstname":"Tom","Constituency_Number":"2","Party_Name":"Labour Party","Candidate_Id":"12","Count_Number":"3","Transfers":"3.942","id":18,"Total_Votes":"1701.942"},</v>
+        <v>{"Candidate_First_Pref_Votes":"1679","Status":"","Occurred_On_Count":"","Surname":"MCINALLY","Firstname":"Tom","Constituency_Number":"2","Party_Name":"Labour Party","Candidate_Id":"12","Count_Number":"3","Transfers":"3.942","id":15,"Total_Votes":"1701.942"},</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="3"/>
-        <v>{"Candidate_First_Pref_Votes":"1679","Status":"","Occurred_On_Count":"","Surname":"MCINALLY","Firstname":"Tom","Constituency_Number":"2","Party_Name":"Labour Party","Candidate_Id":"12","Count_Number":"5","Transfers":"181.55373","id":18,"Total_Votes":"1883.86526"},</v>
+        <v>{"Candidate_First_Pref_Votes":"1679","Status":"","Occurred_On_Count":"","Surname":"MCINALLY","Firstname":"Tom","Constituency_Number":"2","Party_Name":"Labour Party","Candidate_Id":"12","Count_Number":"4","Transfers":"181.55373","id":21,"Total_Votes":"1883.86526"},</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -786,11 +786,11 @@
       </c>
       <c r="G13" t="str">
         <f t="shared" si="2"/>
-        <v>{"Candidate_First_Pref_Votes":"161","Status":"","Occurred_On_Count":"","Surname":"NISBET","Firstname":"James","Constituency_Number":"2","Party_Name":"UK Independence Party (UKIP)","Candidate_Id":"13","Count_Number":"3","Transfers":"","id":19,"Total_Votes":""},</v>
+        <v>{"Candidate_First_Pref_Votes":"161","Status":"","Occurred_On_Count":"","Surname":"NISBET","Firstname":"James","Constituency_Number":"2","Party_Name":"UK Independence Party (UKIP)","Candidate_Id":"13","Count_Number":"3","Transfers":"","id":16,"Total_Votes":""},</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="3"/>
-        <v>{"Candidate_First_Pref_Votes":"161","Status":"","Occurred_On_Count":"","Surname":"NISBET","Firstname":"James","Constituency_Number":"2","Party_Name":"UK Independence Party (UKIP)","Candidate_Id":"13","Count_Number":"5","Transfers":"","id":19,"Total_Votes":""},</v>
+        <v>{"Candidate_First_Pref_Votes":"161","Status":"","Occurred_On_Count":"","Surname":"NISBET","Firstname":"James","Constituency_Number":"2","Party_Name":"UK Independence Party (UKIP)","Candidate_Id":"13","Count_Number":"4","Transfers":"","id":22,"Total_Votes":""},</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -807,11 +807,11 @@
       </c>
       <c r="G14" t="str">
         <f t="shared" si="2"/>
-        <v>{"Candidate_First_Pref_Votes":"2032","Status":"","Occurred_On_Count":"","Surname":"ROSS","Firstname":"Frank","Constituency_Number":"2","Party_Name":"Scottish National Party (SNP)","Candidate_Id":"14","Count_Number":"3","Transfers":"2.7156","id":20,"Total_Votes":"2055.7156"},</v>
+        <v>{"Candidate_First_Pref_Votes":"2032","Status":"","Occurred_On_Count":"","Surname":"ROSS","Firstname":"Frank","Constituency_Number":"2","Party_Name":"Scottish National Party (SNP)","Candidate_Id":"14","Count_Number":"3","Transfers":"2.7156","id":17,"Total_Votes":"2055.7156"},</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="3"/>
-        <v>{"Candidate_First_Pref_Votes":"2032","Status":"","Occurred_On_Count":"","Surname":"ROSS","Firstname":"Frank","Constituency_Number":"2","Party_Name":"Scottish National Party (SNP)","Candidate_Id":"14","Count_Number":"5","Transfers":"0","id":20,"Total_Votes":"2054"},</v>
+        <v>{"Candidate_First_Pref_Votes":"2032","Status":"","Occurred_On_Count":"","Surname":"ROSS","Firstname":"Frank","Constituency_Number":"2","Party_Name":"Scottish National Party (SNP)","Candidate_Id":"14","Count_Number":"4","Transfers":"0","id":23,"Total_Votes":"2054"},</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>